<commit_message>
adding misc Win10 pro defaults
</commit_message>
<xml_diff>
--- a/Win10_Pro-Default_files_directories.xlsx
+++ b/Win10_Pro-Default_files_directories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flakes/code/OS-defaults_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1422A10-9E2F-4542-8580-5F1E48C3484A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFF18A2-EDF3-EF45-A23F-C2F41F7E6CF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33920" yWindow="6320" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{527565E3-21E6-9B4D-B85E-635D2894B5D6}"/>
+    <workbookView xWindow="-39760" yWindow="7260" windowWidth="28040" windowHeight="17440" xr2:uid="{527565E3-21E6-9B4D-B85E-635D2894B5D6}"/>
   </bookViews>
   <sheets>
     <sheet name="System drive default dirs" sheetId="5" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="242">
   <si>
     <t>bfsvc.exe</t>
   </si>
@@ -758,9 +758,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>bootmgr</t>
@@ -1144,7 +1141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6238415A-3800-E740-B4D0-971B750DB4C5}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
@@ -1248,7 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26800F26-EFDA-9440-BBA0-9E5DFC5A5D62}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
@@ -1268,7 +1265,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B2" t="s">
         <v>236</v>
@@ -1276,7 +1273,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B3" t="s">
         <v>236</v>
@@ -1284,7 +1281,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B4" t="s">
         <v>236</v>
@@ -1292,7 +1289,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B5" t="s">
         <v>236</v>
@@ -1300,7 +1297,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B6" t="s">
         <v>236</v>
@@ -1451,8 +1448,8 @@
   <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1637,7 +1634,7 @@
         <v>233</v>
       </c>
       <c r="B33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1885,7 +1882,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>